<commit_message>
BOM Loop PDF file
</commit_message>
<xml_diff>
--- a/Instructions/BOM Loop.xlsx
+++ b/Instructions/BOM Loop.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Pierre\Documents\GitHub\Loop-automatization-Mod\Instructions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B20468-3C2A-413B-AA86-396227F9AD80}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8211F34A-0E71-4B4C-BF58-C914B2D3602F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="28800" windowHeight="12360" xr2:uid="{5E82EB64-A294-4C7B-8DB9-F7B2F90E5586}"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="28800" windowHeight="12360" xr2:uid="{5E82EB64-A294-4C7B-8DB9-F7B2F90E5586}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,7 +183,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -191,11 +191,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -203,6 +218,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -612,7 +631,7 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,230 +658,241 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5" s="3">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="A6" s="3">
+        <v>1</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="A7" s="3">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="A9" s="3">
+        <v>1</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="A10" s="3">
+        <v>1</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="A11" s="3">
+        <v>1</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="A12" s="3">
+        <v>1</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="A13" s="3">
+        <v>1</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="4" t="s">
         <v>34</v>
       </c>
     </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+    </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="A16" s="3">
         <v>16</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="A17" s="3">
         <v>5</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="A18" s="3">
         <v>3</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="A19" s="3">
         <v>14</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="A20" s="3">
+        <v>1</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="A21" s="3">
         <v>2</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>1</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="A22" s="3">
+        <v>1</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="A23" s="3">
+        <v>1</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="4" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+      <c r="A24" s="3">
         <v>6</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="A25" s="3">
         <v>6</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>1</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="A26" s="3">
+        <v>1</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+      <c r="A27" s="3">
         <v>4</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -877,6 +907,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>